<commit_message>
add submission4g script, modified translate batch, and tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -123,12 +123,18 @@
   </si>
   <si>
     <t>MLP, a=0.001, hidden layer 100,100</t>
+  </si>
+  <si>
+    <t>Include num 300</t>
+  </si>
+  <si>
+    <t>max depth 150</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -170,17 +176,17 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -188,6 +194,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -266,6 +277,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -300,6 +312,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -488,38 +501,44 @@
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="B1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>5000</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4">
         <v>10000</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="5">
         <v>300</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="2">
+      <c r="H2" s="5"/>
+      <c r="I2" s="4">
         <v>500</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2" s="4"/>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -533,133 +552,133 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>0.87557238464247999</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>0.87528671964028804</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0.87398731947869002</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>0.87379538058054895</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>0.87463424685761404</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0.87509857057266005</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>0.874098495775809</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>0.87453868438207405</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>0.93094831789371002</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>0.93084372259181303</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>0.84332101372756096</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>0.84015406780158097</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>0.92749090661862199</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>0.92687579564760902</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>0.88222222222222202</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>0.88342109937312696</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <v>0.97821871223405799</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>0.977533997395854</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:13">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>0.97162102473498202</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>0.97125797553499305</v>
       </c>
       <c r="D17">
@@ -669,14 +688,14 @@
         <v>0.97157932071122999</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <v>0.74482145126445498</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>0.743719437257234</v>
       </c>
       <c r="D18">
@@ -697,15 +716,27 @@
       <c r="J18">
         <v>0.742125664479654</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>0.76756894141568099</v>
+      </c>
+      <c r="L18">
+        <v>0.76661235773704395</v>
+      </c>
+      <c r="M18">
+        <v>0.77163553183377798</v>
+      </c>
+      <c r="N18">
+        <v>0.77071145014398701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="3">
         <v>0.85101387406616802</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>0.83954207648014401</v>
       </c>
       <c r="D19">
@@ -715,14 +746,14 @@
         <v>0.90269694587079596</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="3">
         <v>0.63639551192145905</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>0.63210637897517896</v>
       </c>
       <c r="D20">
@@ -732,14 +763,14 @@
         <v>0.88408631561280204</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="3">
         <v>0.984520123839009</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>0.98391572949121098</v>
       </c>
       <c r="D21">
@@ -749,14 +780,14 @@
         <v>0.98409589093219496</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="3">
         <v>0.85127405096203801</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>0.82461934187474195</v>
       </c>
       <c r="D22">
@@ -766,14 +797,14 @@
         <v>0.82382861652051698</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="3">
         <v>0.63982581155977802</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>0.63198404633928995</v>
       </c>
       <c r="D23">
@@ -783,14 +814,14 @@
         <v>0.94731663210621797</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="3">
         <v>0.82601520598809397</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>0.823090635323941</v>
       </c>
       <c r="D24">
@@ -800,7 +831,7 @@
         <v>0.82496450255665299</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -817,7 +848,7 @@
         <v>0.90755273988090002</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -846,7 +877,7 @@
         <v>0.67519265100110604</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -863,7 +894,7 @@
         <v>0.75656608355821398</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -871,7 +902,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -891,7 +922,7 @@
         <v>0.68687521422635001</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -911,7 +942,7 @@
         <v>0.59925360436648301</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1152,7 +1183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1169,14 +1200,14 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="4">
         <v>5000</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4">
         <v>10000</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -1193,7 +1224,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1201,15 +1232,15 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -1227,7 +1258,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1235,39 +1266,39 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1275,57 +1306,57 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">

</xml_diff>

<commit_message>
update tuning and submission7
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -129,13 +129,16 @@
   </si>
   <si>
     <t>max depth 150</t>
+  </si>
+  <si>
+    <t>max depth 130</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -151,6 +154,11 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,6 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -277,7 +286,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,7 +320,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,11 +495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -501,14 +508,14 @@
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -537,8 +544,11 @@
       <c r="M2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -552,12 +562,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -574,7 +584,7 @@
         <v>0.87379538058054895</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -591,27 +601,39 @@
         <v>0.87453868438207405</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="B9" s="6">
+        <v>0.86252354048964197</v>
+      </c>
+      <c r="C9">
+        <v>0.86179557047234701</v>
+      </c>
+      <c r="M9">
+        <v>0.86209553158705698</v>
+      </c>
+      <c r="N9">
+        <v>0.86141106017732105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -622,7 +644,7 @@
         <v>0.93084372259181303</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -633,7 +655,7 @@
         <v>0.84015406780158097</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -644,7 +666,7 @@
         <v>0.92687579564760902</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -655,7 +677,7 @@
         <v>0.88342109937312696</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -666,12 +688,12 @@
         <v>0.977533997395854</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -688,7 +710,7 @@
         <v>0.97157932071122999</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -729,7 +751,7 @@
         <v>0.77071145014398701</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -746,7 +768,7 @@
         <v>0.90269694587079596</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -763,7 +785,7 @@
         <v>0.88408631561280204</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -780,7 +802,7 @@
         <v>0.98409589093219496</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -797,7 +819,7 @@
         <v>0.82382861652051698</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -814,7 +836,7 @@
         <v>0.94731663210621797</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -830,8 +852,20 @@
       <c r="E24">
         <v>0.82496450255665299</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="M24">
+        <v>0.83414864148052104</v>
+      </c>
+      <c r="N24">
+        <v>0.831035375138096</v>
+      </c>
+      <c r="O24">
+        <v>0.83491483467908201</v>
+      </c>
+      <c r="P24">
+        <v>0.83206251620696403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -848,7 +882,7 @@
         <v>0.90755273988090002</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -877,7 +911,7 @@
         <v>0.67519265100110604</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -894,7 +928,7 @@
         <v>0.75656608355821398</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -902,7 +936,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -922,7 +956,7 @@
         <v>0.68687521422635001</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -942,7 +976,7 @@
         <v>0.59925360436648301</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1183,7 +1217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
update tuning results and testtest
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Random Forest" sheetId="1" r:id="rId1"/>
-    <sheet name="Logistic" sheetId="2" r:id="rId2"/>
+    <sheet name="Best" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>max depth 100</t>
+  </si>
+  <si>
+    <t>maxdepth150,minsplit=6</t>
+  </si>
+  <si>
+    <t>include dot + combine inch</t>
+  </si>
+  <si>
+    <t>include dot</t>
+  </si>
+  <si>
+    <t>combine vneck</t>
+  </si>
+  <si>
+    <t>Remove everyother number labels except self</t>
   </si>
 </sst>
 </file>
@@ -184,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +214,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -511,14 +529,14 @@
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -553,8 +571,11 @@
       <c r="Q2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="S2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -568,12 +589,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -590,7 +611,7 @@
         <v>0.87379538058054895</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -607,17 +628,17 @@
         <v>0.87453868438207405</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -634,12 +655,12 @@
         <v>0.86141106017732105</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -650,7 +671,7 @@
         <v>0.93084372259181303</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -661,7 +682,7 @@
         <v>0.84015406780158097</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -672,7 +693,7 @@
         <v>0.92687579564760902</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -683,7 +704,7 @@
         <v>0.88342109937312696</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -694,7 +715,7 @@
         <v>0.977533997395854</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -947,6 +968,9 @@
       <c r="E29" t="s">
         <v>32</v>
       </c>
+      <c r="I29" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
@@ -967,6 +991,15 @@
       <c r="G30">
         <v>0.68687521422635001</v>
       </c>
+      <c r="I30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30">
+        <v>0.77152469796604894</v>
+      </c>
+      <c r="K30">
+        <v>0.76812539883812503</v>
+      </c>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
@@ -987,6 +1020,15 @@
       <c r="G31">
         <v>0.59925360436648301</v>
       </c>
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <v>0.90693703308431095</v>
+      </c>
+      <c r="K31">
+        <v>0.90055440230551198</v>
+      </c>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
@@ -1007,16 +1049,28 @@
       <c r="G32">
         <v>0.66857234277294697</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="I32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32">
+        <v>0.88674614305750299</v>
+      </c>
+      <c r="K32">
+        <v>0.88535929463632401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>29</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="I34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1035,8 +1089,17 @@
       <c r="G35">
         <v>0.747028181293104</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="I35" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35">
+        <v>0.77228934087780998</v>
+      </c>
+      <c r="K35">
+        <v>0.76900154145400901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1055,8 +1118,17 @@
       <c r="G36">
         <v>0.66242462371928501</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>0.90736392742796101</v>
+      </c>
+      <c r="K36">
+        <v>0.90106841717018604</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -1075,16 +1147,28 @@
       <c r="G37">
         <v>0.73758601868260398</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="I37" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37">
+        <v>0.88551893408134597</v>
+      </c>
+      <c r="K37">
+        <v>0.88397733518379495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>30</v>
       </c>
       <c r="E39" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="I39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1103,8 +1187,17 @@
       <c r="G40">
         <v>0.75250686533970801</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40">
+        <v>0.93466209081309304</v>
+      </c>
+      <c r="K40">
+        <v>0.93246486531728501</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1124,7 +1217,7 @@
         <v>0.66466851909281899</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -1143,16 +1236,33 @@
       <c r="G42">
         <v>0.734000645409841</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="I42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="I43" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43">
+        <v>0.77228934087780998</v>
+      </c>
+      <c r="K43">
+        <v>0.76900154145400901</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>31</v>
       </c>
       <c r="E44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1171,8 +1281,11 @@
       <c r="G45">
         <v>0.73164397213811105</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1192,7 +1305,7 @@
         <v>0.631103221363433</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1346,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1243,17 +1356,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5">
-        <v>5000</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5">
-        <v>10000</v>
-      </c>
-      <c r="E1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -1262,12 +1368,6 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
@@ -1420,10 +1520,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>

</xml_diff>

<commit_message>
Update finals scripts, english translation (In progress) and tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -153,13 +153,19 @@
   </si>
   <si>
     <t>~70</t>
+  </si>
+  <si>
+    <t>gini</t>
+  </si>
+  <si>
+    <t>entropy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -182,12 +188,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -202,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,7 +223,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -221,6 +232,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,6 +325,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -344,6 +360,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -519,49 +536,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19"/>
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>5000</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
         <v>10000</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="5"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>300</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6">
+      <c r="H2" s="6"/>
+      <c r="I2" s="5">
         <v>500</v>
       </c>
-      <c r="J2" s="6"/>
+      <c r="J2" s="5"/>
       <c r="K2" t="s">
         <v>36</v>
       </c>
@@ -578,7 +595,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -592,12 +609,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -613,8 +630,14 @@
       <c r="E5" s="3">
         <v>0.87379538058054895</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="S5" s="10">
+        <v>0.883629799225079</v>
+      </c>
+      <c r="T5" s="10">
+        <v>0.88351498780051996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -631,24 +654,30 @@
         <v>0.87453868438207405</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="B8" s="8">
+        <v>0.98935712969974798</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.98935279738664506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="9">
         <v>0.86252354048964197</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>0.86179557047234701</v>
       </c>
       <c r="M9">
@@ -658,12 +687,12 @@
         <v>0.86141106017732105</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -674,7 +703,7 @@
         <v>0.93084372259181303</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -685,7 +714,7 @@
         <v>0.84015406780158097</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -696,7 +725,7 @@
         <v>0.92687579564760902</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -707,7 +736,7 @@
         <v>0.88342109937312696</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -718,12 +747,12 @@
         <v>0.977533997395854</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -740,7 +769,7 @@
         <v>0.97157932071122999</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -781,7 +810,7 @@
         <v>0.77071145014398701</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -798,7 +827,7 @@
         <v>0.90269694587079596</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -815,7 +844,7 @@
         <v>0.88408631561280204</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -832,7 +861,7 @@
         <v>0.98409589093219496</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -849,7 +878,7 @@
         <v>0.82382861652051698</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -866,7 +895,7 @@
         <v>0.94731663210621797</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -901,7 +930,7 @@
         <v>0.83105263632751003</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -918,7 +947,7 @@
         <v>0.90755273988090002</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -947,7 +976,7 @@
         <v>0.67519265100110604</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -964,7 +993,7 @@
         <v>0.75656608355821398</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -974,8 +1003,14 @@
       <c r="I29" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="L29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1003,8 +1038,17 @@
       <c r="K30">
         <v>0.76812539883812503</v>
       </c>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="O30" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P30" s="10">
+        <v>0.884906657273687</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>0.884801461445482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1032,8 +1076,9 @@
       <c r="K31">
         <v>0.90055440230551198</v>
       </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1062,7 +1107,7 @@
         <v>0.88535929463632401</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1072,8 +1117,14 @@
       <c r="I34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="J34" t="s">
+        <v>47</v>
+      </c>
+      <c r="L34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1092,7 +1143,7 @@
       <c r="G35">
         <v>0.747028181293104</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J35">
@@ -1101,8 +1152,14 @@
       <c r="K35">
         <v>0.76900154145400901</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" s="7">
+        <v>0.77718305551307498</v>
+      </c>
+      <c r="M35" s="7">
+        <v>0.77410656270602296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1178,7 @@
       <c r="G36">
         <v>0.66242462371928501</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J36">
@@ -1130,8 +1187,14 @@
       <c r="K36">
         <v>0.90106841717018604</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" s="7">
+        <v>0.909498399146211</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0.90355579484173498</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -1160,7 +1223,18 @@
         <v>0.88397733518379495</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I38" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38" s="10">
+        <v>0.95059382422802796</v>
+      </c>
+      <c r="M38" s="10">
+        <v>0.95020848780309397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1171,7 +1245,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1274,7 @@
         <v>0.93246486531728501</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1220,7 +1294,7 @@
         <v>0.66466851909281899</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -1243,7 +1317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I43" t="s">
         <v>27</v>
       </c>
@@ -1254,7 +1328,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1271,7 +1345,7 @@
         <v>0.87960055180985197</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1300,7 +1374,7 @@
         <v>0.85021390020914001</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1320,7 +1394,7 @@
         <v>0.631103221363433</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -1357,26 +1431,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5703125"/>
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1384,152 +1458,152 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
optimized final scripts by adding unrelated text filters, added word frequency analysis scripts and results, and update tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="52">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -165,13 +165,19 @@
   </si>
   <si>
     <t>don’t include dot, max depth 150, entropy</t>
+  </si>
+  <si>
+    <t>remove promo</t>
+  </si>
+  <si>
+    <t>remove mobile test filter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -220,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,6 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,6 +338,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -365,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,27 +549,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19"/>
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -599,7 +608,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -613,12 +622,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -641,7 +650,7 @@
         <v>0.88351498780051996</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -658,12 +667,12 @@
         <v>0.87453868438207405</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -674,7 +683,7 @@
         <v>0.98935279738664506</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -691,12 +700,12 @@
         <v>0.86141106017732105</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -707,7 +716,7 @@
         <v>0.93084372259181303</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -718,7 +727,7 @@
         <v>0.84015406780158097</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -729,7 +738,7 @@
         <v>0.92687579564760902</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -740,7 +749,7 @@
         <v>0.88342109937312696</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -751,12 +760,12 @@
         <v>0.977533997395854</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -773,7 +782,7 @@
         <v>0.97157932071122999</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -814,7 +823,7 @@
         <v>0.77071145014398701</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -831,7 +840,7 @@
         <v>0.90269694587079596</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -848,7 +857,7 @@
         <v>0.88408631561280204</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -865,7 +874,7 @@
         <v>0.98409589093219496</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -882,7 +891,7 @@
         <v>0.82382861652051698</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -899,7 +908,7 @@
         <v>0.94731663210621797</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -934,7 +943,7 @@
         <v>0.83105263632751003</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -951,7 +960,7 @@
         <v>0.90755273988090002</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -980,7 +989,7 @@
         <v>0.67519265100110604</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -997,7 +1006,7 @@
         <v>0.75656608355821398</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>0.884801461445482</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1082,7 +1091,7 @@
       </c>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1111,7 +1120,7 @@
         <v>0.88535929463632401</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1128,7 +1137,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1147,23 +1156,23 @@
       <c r="G35">
         <v>0.747028181293104</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="11">
         <v>0.77228934087780998</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="11">
         <v>0.76900154145400901</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L35" s="11">
         <v>0.77718305551307498</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M35" s="11">
         <v>0.77410656270602296</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1182,7 +1191,7 @@
       <c r="G36">
         <v>0.66242462371928501</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="I36" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J36">
@@ -1191,14 +1200,14 @@
       <c r="K36">
         <v>0.90106841717018604</v>
       </c>
-      <c r="L36" s="5">
+      <c r="L36" s="11">
         <v>0.909498399146211</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="11">
         <v>0.90355579484173498</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>0.88397733518379495</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I38" s="8" t="s">
         <v>23</v>
       </c>
@@ -1238,7 +1247,7 @@
         <v>0.95020848780309397</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1278,7 +1287,7 @@
         <v>0.93246486531728501</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>0.66466851909281899</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I43" t="s">
         <v>27</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>0.87960055180985197</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>0.85021390020914001</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>0.631103221363433</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>0.72563454180971099</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B50" s="8" t="s">
         <v>42</v>
       </c>
@@ -1427,19 +1436,34 @@
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="I50" t="s">
+        <v>50</v>
+      </c>
+      <c r="K50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="5">
         <v>0.972173144876325</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="5">
         <v>0.97179325336495403</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="H51" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51">
+        <v>0.97173144876325002</v>
+      </c>
+      <c r="L51">
+        <v>0.97123473865937504</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>19</v>
       </c>
@@ -1452,23 +1476,59 @@
       <c r="D52" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="H52" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" s="5">
+        <v>0.77138136993264705</v>
+      </c>
+      <c r="L52" s="5">
+        <v>0.77026625297587303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="H53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="5">
+        <v>0.91056563500533605</v>
+      </c>
+      <c r="L53" s="5">
+        <v>0.90479330659597801</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="H54" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54">
+        <v>0.890778401122019</v>
+      </c>
+      <c r="J54">
+        <v>0.88934764022218704</v>
+      </c>
+      <c r="K54" s="5">
+        <v>0.89042776998597395</v>
+      </c>
+      <c r="L54" s="5">
+        <v>0.88911397041819495</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="H55" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>22</v>
       </c>
@@ -1478,13 +1538,37 @@
       <c r="C56" s="8">
         <v>0.82813047025675701</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="H56" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="5">
+        <v>0.85761830473218903</v>
+      </c>
+      <c r="J56" s="5">
+        <v>0.82888401632192199</v>
+      </c>
+      <c r="K56" s="11">
+        <v>0.85678627145085795</v>
+      </c>
+      <c r="L56" s="11">
+        <v>0.82753126240531305</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="H57" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="5">
+        <v>0.95130641330166199</v>
+      </c>
+      <c r="L57" s="5">
+        <v>0.95093413607259503</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>24</v>
       </c>
@@ -1494,20 +1578,56 @@
       <c r="C58" s="8">
         <v>0.83846606975927196</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="H58" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K58" s="5">
+        <v>0.84169269758943799</v>
+      </c>
+      <c r="L58" s="5">
+        <v>0.83904685698053205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="H59" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="H60" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K60" s="5">
+        <v>0.69987799918666105</v>
+      </c>
+      <c r="L60" s="5">
+        <v>0.69390833463344603</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>27</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0.77718305551307498</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0.77410656270602296</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K61">
+        <v>0.776571341183667</v>
+      </c>
+      <c r="L61">
+        <v>0.77373729773394795</v>
       </c>
     </row>
   </sheetData>
@@ -1527,26 +1647,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5703125"/>
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1554,152 +1674,152 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
added combined script for beauty and mobile brand and update tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -170,14 +170,53 @@
     <t>remove promo</t>
   </si>
   <si>
-    <t>remove mobile test filter</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>300tree, gini, minsplit 6, include numdot</t>
+  </si>
+  <si>
+    <t>remove mobile filter (pre)</t>
+  </si>
+  <si>
+    <t>remove mobile filter (post)</t>
+  </si>
+  <si>
+    <t>replace krem, combine naturerepublic (pre)</t>
+  </si>
+  <si>
+    <t>replace krem, combine naturerepublic (post)</t>
+  </si>
+  <si>
+    <t>remove beauty filter</t>
+  </si>
+  <si>
+    <t>maxdepth100</t>
+  </si>
+  <si>
+    <t>maxdepth110</t>
+  </si>
+  <si>
+    <t>maxdepth120</t>
+  </si>
+  <si>
+    <t>maxdepth130</t>
+  </si>
+  <si>
+    <t>maxdepth140</t>
+  </si>
+  <si>
+    <t>maxdepth150</t>
+  </si>
+  <si>
+    <t>300tree, gini, minsplit 6, filter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -242,13 +281,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,7 +377,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -373,7 +411,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,49 +586,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19"/>
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="10">
         <v>5000</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10">
         <v>10000</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="10"/>
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="11">
         <v>300</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="9">
+      <c r="H2" s="11"/>
+      <c r="I2" s="10">
         <v>500</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="10"/>
       <c r="K2" t="s">
         <v>36</v>
       </c>
@@ -608,7 +645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -622,12 +659,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -650,7 +687,7 @@
         <v>0.88351498780051996</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -667,12 +704,12 @@
         <v>0.87453868438207405</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -683,7 +720,7 @@
         <v>0.98935279738664506</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -700,12 +737,15 @@
         <v>0.86141106017732105</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -716,7 +756,7 @@
         <v>0.93084372259181303</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -726,8 +766,14 @@
       <c r="C12" s="3">
         <v>0.84015406780158097</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E12" s="5">
+        <v>0.93466209081309304</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.93246486531728501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -738,7 +784,7 @@
         <v>0.92687579564760902</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -749,7 +795,7 @@
         <v>0.88342109937312696</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -760,12 +806,12 @@
         <v>0.977533997395854</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -782,7 +828,7 @@
         <v>0.97157932071122999</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -823,7 +869,7 @@
         <v>0.77071145014398701</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -840,7 +886,7 @@
         <v>0.90269694587079596</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -857,7 +903,7 @@
         <v>0.88408631561280204</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -874,7 +920,7 @@
         <v>0.98409589093219496</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -891,7 +937,7 @@
         <v>0.82382861652051698</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -908,7 +954,7 @@
         <v>0.94731663210621797</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -943,7 +989,7 @@
         <v>0.83105263632751003</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -960,7 +1006,7 @@
         <v>0.90755273988090002</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -989,7 +1035,7 @@
         <v>0.67519265100110604</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1006,7 +1052,7 @@
         <v>0.75656608355821398</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1023,7 +1069,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1107,7 @@
         <v>0.884801461445482</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1091,7 +1137,7 @@
       </c>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1120,7 +1166,7 @@
         <v>0.88535929463632401</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1156,23 +1202,23 @@
       <c r="G35">
         <v>0.747028181293104</v>
       </c>
-      <c r="I35" s="11" t="s">
+      <c r="I35" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J35" s="11">
+      <c r="J35" s="9">
         <v>0.77228934087780998</v>
       </c>
-      <c r="K35" s="11">
+      <c r="K35" s="9">
         <v>0.76900154145400901</v>
       </c>
-      <c r="L35" s="11">
+      <c r="L35" s="9">
         <v>0.77718305551307498</v>
       </c>
-      <c r="M35" s="11">
+      <c r="M35" s="9">
         <v>0.77410656270602296</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1191,7 +1237,7 @@
       <c r="G36">
         <v>0.66242462371928501</v>
       </c>
-      <c r="I36" s="11" t="s">
+      <c r="I36" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J36">
@@ -1200,14 +1246,14 @@
       <c r="K36">
         <v>0.90106841717018604</v>
       </c>
-      <c r="L36" s="11">
+      <c r="L36" s="9">
         <v>0.909498399146211</v>
       </c>
-      <c r="M36" s="11">
+      <c r="M36" s="9">
         <v>0.90355579484173498</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -1236,7 +1282,7 @@
         <v>0.88397733518379495</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="I38" s="8" t="s">
         <v>23</v>
       </c>
@@ -1247,18 +1293,15 @@
         <v>0.95020848780309397</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>30</v>
       </c>
       <c r="E39" t="s">
         <v>34</v>
       </c>
-      <c r="I39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1277,17 +1320,8 @@
       <c r="G40">
         <v>0.75250686533970801</v>
       </c>
-      <c r="I40" t="s">
-        <v>13</v>
-      </c>
-      <c r="J40">
-        <v>0.93466209081309304</v>
-      </c>
-      <c r="K40">
-        <v>0.93246486531728501</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1307,7 +1341,7 @@
         <v>0.66466851909281899</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -1330,7 +1364,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="I43" t="s">
         <v>27</v>
       </c>
@@ -1341,7 +1375,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1358,7 +1392,7 @@
         <v>0.87960055180985197</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1387,7 +1421,7 @@
         <v>0.85021390020914001</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -1407,7 +1441,7 @@
         <v>0.631103221363433</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -1427,7 +1461,7 @@
         <v>0.72563454180971099</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="B50" s="8" t="s">
         <v>42</v>
       </c>
@@ -1439,11 +1473,14 @@
       <c r="I50" t="s">
         <v>50</v>
       </c>
-      <c r="K50" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K50" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="8" t="s">
         <v>18</v>
       </c>
@@ -1462,8 +1499,14 @@
       <c r="L51">
         <v>0.97123473865937504</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51">
+        <v>0.97184187279151901</v>
+      </c>
+      <c r="N51">
+        <v>0.97136146546973201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="8" t="s">
         <v>19</v>
       </c>
@@ -1479,28 +1522,40 @@
       <c r="H52" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K52" s="5">
+      <c r="K52" s="9">
         <v>0.77138136993264705</v>
       </c>
-      <c r="L52" s="5">
+      <c r="L52" s="9">
         <v>0.77026625297587303</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" s="5">
+        <v>0.77201677468547403</v>
+      </c>
+      <c r="N52" s="5">
+        <v>0.77080676283850602</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K53" s="5">
+      <c r="K53" s="9">
         <v>0.91056563500533605</v>
       </c>
-      <c r="L53" s="5">
+      <c r="L53" s="9">
         <v>0.90479330659597801</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" s="5">
+        <v>0.91120597652081103</v>
+      </c>
+      <c r="N53" s="5">
+        <v>0.90555717310919603</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" s="8" t="s">
         <v>21</v>
       </c>
@@ -1519,8 +1574,14 @@
       <c r="L54" s="5">
         <v>0.88911397041819495</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54">
+        <v>0.89007713884992901</v>
+      </c>
+      <c r="N54">
+        <v>0.88877534813885395</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" s="8" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14">
       <c r="A56" s="8" t="s">
         <v>22</v>
       </c>
@@ -1541,20 +1602,26 @@
       <c r="H56" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I56" s="9">
         <v>0.85761830473218903</v>
       </c>
-      <c r="J56" s="5">
+      <c r="J56" s="9">
         <v>0.82888401632192199</v>
       </c>
-      <c r="K56" s="11">
+      <c r="K56" s="9">
         <v>0.85678627145085795</v>
       </c>
-      <c r="L56" s="11">
+      <c r="L56" s="9">
         <v>0.82753126240531305</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" s="5">
+        <v>0.85772230889235501</v>
+      </c>
+      <c r="N56" s="5">
+        <v>0.82871303579287103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="8" t="s">
         <v>23</v>
       </c>
@@ -1567,8 +1634,14 @@
       <c r="L57" s="5">
         <v>0.95093413607259503</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" s="9">
+        <v>0.95106888361045105</v>
+      </c>
+      <c r="N57" s="9">
+        <v>0.95069044895470201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="8" t="s">
         <v>24</v>
       </c>
@@ -1581,14 +1654,20 @@
       <c r="H58" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K58" s="5">
+      <c r="K58" s="9">
         <v>0.84169269758943799</v>
       </c>
-      <c r="L58" s="5">
+      <c r="L58" s="9">
         <v>0.83904685698053205</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" s="5">
+        <v>0.84393233924677302</v>
+      </c>
+      <c r="N58" s="5">
+        <v>0.84133483164585698</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="8" t="s">
         <v>25</v>
       </c>
@@ -1596,7 +1675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="A60" s="8" t="s">
         <v>26</v>
       </c>
@@ -1609,15 +1688,21 @@
       <c r="L60" s="5">
         <v>0.69390833463344603</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60">
+        <v>0.69621797478649805</v>
+      </c>
+      <c r="N60">
+        <v>0.68982351609072101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="9">
         <v>0.77718305551307498</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="9">
         <v>0.77410656270602296</v>
       </c>
       <c r="H61" s="8" t="s">
@@ -1628,6 +1713,321 @@
       </c>
       <c r="L61">
         <v>0.77373729773394795</v>
+      </c>
+      <c r="M61" s="5">
+        <v>0.77871234133659495</v>
+      </c>
+      <c r="N61" s="5">
+        <v>0.77590760363536704</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="9">
+        <v>0.88499471644945404</v>
+      </c>
+      <c r="C66" s="9">
+        <v>0.88493682414062602</v>
+      </c>
+      <c r="F66" s="8">
+        <v>0.88437830221909097</v>
+      </c>
+      <c r="G66" s="8">
+        <v>0.88430830938662097</v>
+      </c>
+      <c r="J66" s="8">
+        <v>0.88437830221909097</v>
+      </c>
+      <c r="K66" s="8">
+        <v>0.88432641588155902</v>
+      </c>
+      <c r="M66" s="5">
+        <v>0.88530292356463502</v>
+      </c>
+      <c r="N66" s="5">
+        <v>0.88524550220276998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="8">
+        <v>0.88093962497424205</v>
+      </c>
+      <c r="C67" s="8">
+        <v>0.88172387460379997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M69" s="8">
+        <v>0.989561800282445</v>
+      </c>
+      <c r="N69" s="8">
+        <v>0.98955582520563601</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="8">
+        <v>0.86834446156480005</v>
+      </c>
+      <c r="C70">
+        <v>0.86750806166279304</v>
+      </c>
+      <c r="J70" s="8">
+        <v>0.86902927580893596</v>
+      </c>
+      <c r="K70">
+        <v>0.86824548783136801</v>
+      </c>
+      <c r="M70" s="8">
+        <v>0.86877247046738504</v>
+      </c>
+      <c r="N70" s="8">
+        <v>0.86801224810394795</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J72" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L72" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="8">
+        <v>0.878962662909475</v>
+      </c>
+      <c r="C73" s="8">
+        <v>0.87907604215382595</v>
+      </c>
+      <c r="D73" s="8">
+        <v>0.88045966889749905</v>
+      </c>
+      <c r="E73" s="8">
+        <v>0.88057062396202701</v>
+      </c>
+      <c r="F73" s="8">
+        <v>0.88252905952800198</v>
+      </c>
+      <c r="G73" s="8">
+        <v>0.88261129460746302</v>
+      </c>
+      <c r="H73" s="8">
+        <v>0.88398203592814295</v>
+      </c>
+      <c r="I73" s="8">
+        <v>0.884063230824641</v>
+      </c>
+      <c r="J73" s="8">
+        <v>0.88349771046143</v>
+      </c>
+      <c r="K73" s="8">
+        <v>0.88354589634232295</v>
+      </c>
+      <c r="L73" s="8">
+        <v>0.88345368087354703</v>
+      </c>
+      <c r="M73" s="8">
+        <v>0.88346679477420997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="8">
+        <v>0.86573253657531402</v>
+      </c>
+      <c r="C74" s="8">
+        <v>0.86752989629059996</v>
+      </c>
+      <c r="D74" s="8">
+        <v>0.87088398928497801</v>
+      </c>
+      <c r="E74" s="8">
+        <v>0.87246505703567001</v>
+      </c>
+      <c r="F74" s="8">
+        <v>0.87364516793735802</v>
+      </c>
+      <c r="G74" s="8">
+        <v>0.875119249536222</v>
+      </c>
+      <c r="H74" s="8">
+        <v>0.87710694415825197</v>
+      </c>
+      <c r="I74" s="8">
+        <v>0.878461324297376</v>
+      </c>
+      <c r="J74" s="8">
+        <v>0.87698330929321999</v>
+      </c>
+      <c r="K74" s="8">
+        <v>0.878218642858827</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.87826086956521698</v>
+      </c>
+      <c r="M74" s="8">
+        <v>0.87951075417315405</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="8">
+        <v>0.98232058119514498</v>
+      </c>
+      <c r="C75" s="8">
+        <v>0.98232058119514498</v>
+      </c>
+      <c r="D75" s="8">
+        <v>0.98400033595095104</v>
+      </c>
+      <c r="E75" s="8">
+        <v>0.98288616394453898</v>
+      </c>
+      <c r="F75" s="8">
+        <v>0.98559610296896605</v>
+      </c>
+      <c r="G75" s="8">
+        <v>0.98476342667589201</v>
+      </c>
+      <c r="H75" s="8">
+        <v>0.98616302019905</v>
+      </c>
+      <c r="I75" s="8">
+        <v>0.98540651755862496</v>
+      </c>
+      <c r="J75" s="8">
+        <v>0.98689791290471596</v>
+      </c>
+      <c r="K75" s="8">
+        <v>0.98624389235045895</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="8">
+        <v>0.98868171677684702</v>
+      </c>
+      <c r="C76" s="8">
+        <v>0.98868171677684702</v>
+      </c>
+      <c r="D76" s="8">
+        <v>0.98880451912646505</v>
+      </c>
+      <c r="E76" s="8">
+        <v>0.98879389664129402</v>
+      </c>
+      <c r="F76" s="8">
+        <v>0.98909105794224195</v>
+      </c>
+      <c r="G76" s="8">
+        <v>0.98908210401622199</v>
+      </c>
+      <c r="H76" s="8">
+        <v>0.98917292617532004</v>
+      </c>
+      <c r="I76" s="8">
+        <v>0.98916270072090096</v>
+      </c>
+      <c r="J76" s="8">
+        <v>0.98931619558320805</v>
+      </c>
+      <c r="K76" s="8">
+        <v>0.989307166531181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="8">
+        <v>0.86141071734291996</v>
+      </c>
+      <c r="C77" s="8">
+        <v>0.86067726102978703</v>
+      </c>
+      <c r="D77" s="8">
+        <v>0.86235233692860802</v>
+      </c>
+      <c r="E77" s="8">
+        <v>0.86153961561103598</v>
+      </c>
+      <c r="F77" s="8">
+        <v>0.864321177880499</v>
+      </c>
+      <c r="G77" s="8">
+        <v>0.86364922467519301</v>
+      </c>
+      <c r="H77" s="8">
+        <v>0.86543400102722101</v>
+      </c>
+      <c r="I77" s="8">
+        <v>0.86471262347313105</v>
+      </c>
+      <c r="J77" s="8">
+        <v>0.86629001883239098</v>
+      </c>
+      <c r="K77" s="8">
+        <v>0.86552139689762897</v>
       </c>
     </row>
   </sheetData>
@@ -1647,26 +2047,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="19.5703125"/>
     <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1674,152 +2074,152 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
optimize fashion scripts and update tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>300tree, gini, minsplit 6, filter</t>
+  </si>
+  <si>
+    <t>300tree, gini, minsplit 6</t>
+  </si>
+  <si>
+    <t>add filter</t>
+  </si>
+  <si>
+    <t>addfilter + change v to vneck</t>
   </si>
 </sst>
 </file>
@@ -587,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T77"/>
+  <dimension ref="A1:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2028,6 +2037,105 @@
       </c>
       <c r="K77" s="8">
         <v>0.86552139689762897</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="8">
+        <v>0.93597635299853699</v>
+      </c>
+      <c r="C80">
+        <v>0.93644559215300005</v>
+      </c>
+      <c r="D80" s="5">
+        <v>0.93704290589956096</v>
+      </c>
+      <c r="E80" s="5">
+        <v>0.93760573225891397</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81">
+        <v>0.94319781766983402</v>
+      </c>
+      <c r="C81">
+        <v>0.94191704402598297</v>
+      </c>
+      <c r="D81" s="5">
+        <v>0.94442977824709595</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0.943234103694091</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0.93014243464663204</v>
+      </c>
+      <c r="C82" s="5">
+        <v>0.92945936256083095</v>
+      </c>
+      <c r="D82">
+        <v>0.92993847095216997</v>
+      </c>
+      <c r="E82">
+        <v>0.92924368229589904</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B83">
+        <v>0.88880341880341796</v>
+      </c>
+      <c r="C83">
+        <v>0.89048373759088995</v>
+      </c>
+      <c r="D83" s="5">
+        <v>0.88934472934472897</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0.89108264002774595</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84">
+        <v>0.97880891487029598</v>
+      </c>
+      <c r="C84">
+        <v>0.97820936077994702</v>
+      </c>
+      <c r="D84" s="5">
+        <v>0.97959585171861296</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0.97911882585996102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimize collar type and update tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -599,7 +599,7 @@
   <dimension ref="A1:T84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S65" sqref="S65"/>
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2070,7 +2070,7 @@
         <v>0.93760573225891397</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:7">
       <c r="A81" s="8" t="s">
         <v>13</v>
       </c>
@@ -2080,14 +2080,20 @@
       <c r="C81">
         <v>0.94191704402598297</v>
       </c>
-      <c r="D81" s="5">
+      <c r="D81" s="9">
         <v>0.94442977824709595</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="9">
         <v>0.943234103694091</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" s="5">
+        <v>0.946013727560718</v>
+      </c>
+      <c r="G81" s="5">
+        <v>0.94488480359481897</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="8" t="s">
         <v>14</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>0.92924368229589904</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:7">
       <c r="A83" s="8" t="s">
         <v>15</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>0.89108264002774595</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:7">
       <c r="A84" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
update testtest and tuning results
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="70">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>addfilter + change v to vneck</t>
+  </si>
+  <si>
+    <t>concat all neck</t>
+  </si>
+  <si>
+    <t>concat specific neck + sleeve</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
   <dimension ref="A1:T84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82"/>
+      <selection activeCell="R77" sqref="R77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2052,6 +2058,12 @@
       <c r="F79" s="8" t="s">
         <v>67</v>
       </c>
+      <c r="H79" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J79" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="8" t="s">
@@ -2069,8 +2081,20 @@
       <c r="E80" s="5">
         <v>0.93760573225891397</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80">
+        <v>0.93551925889809795</v>
+      </c>
+      <c r="I80">
+        <v>0.93609947703377405</v>
+      </c>
+      <c r="J80">
+        <v>0.93585446123841998</v>
+      </c>
+      <c r="K80">
+        <v>0.93629975728944603</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="8" t="s">
         <v>13</v>
       </c>
@@ -2092,8 +2116,20 @@
       <c r="G81" s="5">
         <v>0.94488480359481897</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" s="9">
+        <v>0.94491376275959105</v>
+      </c>
+      <c r="I81" s="9">
+        <v>0.94410593043621405</v>
+      </c>
+      <c r="J81" s="8">
+        <v>0.94354980640619501</v>
+      </c>
+      <c r="K81" s="8">
+        <v>0.94251706454765305</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="8" t="s">
         <v>14</v>
       </c>
@@ -2109,8 +2145,14 @@
       <c r="E82">
         <v>0.92924368229589904</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82">
+        <v>0.92915661012339801</v>
+      </c>
+      <c r="I82">
+        <v>0.92850538857704101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="8" t="s">
         <v>15</v>
       </c>
@@ -2126,8 +2168,14 @@
       <c r="E83" s="5">
         <v>0.89108264002774595</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83">
+        <v>0.88985754985754895</v>
+      </c>
+      <c r="I83">
+        <v>0.89164932846988298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="8" t="s">
         <v>16</v>
       </c>
@@ -2137,11 +2185,23 @@
       <c r="C84">
         <v>0.97820936077994702</v>
       </c>
-      <c r="D84" s="5">
+      <c r="D84" s="9">
         <v>0.97959585171861296</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84" s="9">
         <v>0.97911882585996102</v>
+      </c>
+      <c r="H84">
+        <v>0.97976448104325298</v>
+      </c>
+      <c r="I84">
+        <v>0.97927982232396704</v>
+      </c>
+      <c r="J84" s="5">
+        <v>0.98575082206795706</v>
+      </c>
+      <c r="K84" s="5">
+        <v>0.98571397161919105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimized 3 attr from fashion and update tuning results and also latest submission
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -230,7 +230,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -392,6 +392,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -426,6 +427,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -601,11 +603,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R77" sqref="R77"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -781,10 +783,10 @@
       <c r="C12" s="3">
         <v>0.84015406780158097</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="9">
         <v>0.93466209081309304</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="9">
         <v>0.93246486531728501</v>
       </c>
     </row>
@@ -2088,10 +2090,10 @@
         <v>0.93609947703377405</v>
       </c>
       <c r="J80">
-        <v>0.93585446123841998</v>
+        <v>0.93643344709897602</v>
       </c>
       <c r="K80">
-        <v>0.93629975728944603</v>
+        <v>0.93706182620685796</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -2110,10 +2112,10 @@
       <c r="E81" s="9">
         <v>0.943234103694091</v>
       </c>
-      <c r="F81" s="5">
+      <c r="F81" s="9">
         <v>0.946013727560718</v>
       </c>
-      <c r="G81" s="5">
+      <c r="G81" s="9">
         <v>0.94488480359481897</v>
       </c>
       <c r="H81" s="9">
@@ -2122,11 +2124,11 @@
       <c r="I81" s="9">
         <v>0.94410593043621405</v>
       </c>
-      <c r="J81" s="8">
-        <v>0.94354980640619501</v>
-      </c>
-      <c r="K81" s="8">
-        <v>0.94251706454765305</v>
+      <c r="J81" s="5">
+        <v>0.947641675466385</v>
+      </c>
+      <c r="K81" s="5">
+        <v>0.94653712356144004</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -2151,6 +2153,12 @@
       <c r="I82">
         <v>0.92850538857704101</v>
       </c>
+      <c r="J82">
+        <v>0.93000645885032396</v>
+      </c>
+      <c r="K82">
+        <v>0.92929464612063195</v>
+      </c>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="8" t="s">
@@ -2162,10 +2170,10 @@
       <c r="C83">
         <v>0.89048373759088995</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D83" s="9">
         <v>0.88934472934472897</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83" s="9">
         <v>0.89108264002774595</v>
       </c>
       <c r="H83">
@@ -2173,6 +2181,12 @@
       </c>
       <c r="I83">
         <v>0.89164932846988298</v>
+      </c>
+      <c r="J83" s="5">
+        <v>0.88982905982905902</v>
+      </c>
+      <c r="K83" s="5">
+        <v>0.89159668313158402</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -2198,10 +2212,10 @@
         <v>0.97927982232396704</v>
       </c>
       <c r="J84" s="5">
-        <v>0.98575082206795706</v>
+        <v>0.986425339366515</v>
       </c>
       <c r="K84" s="5">
-        <v>0.98571397161919105</v>
+        <v>0.98639262201210398</v>
       </c>
     </row>
   </sheetData>
@@ -2221,7 +2235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
add indonesian stopwords removal and stemming, and update some other misc files
</commit_message>
<xml_diff>
--- a/tuning.xlsx
+++ b/tuning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="345"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="85">
   <si>
     <t>RANDOM FOREST</t>
   </si>
@@ -267,12 +267,15 @@
   </si>
   <si>
     <t>double model 5 fold</t>
+  </si>
+  <si>
+    <t>double model 5 fold iso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -434,6 +437,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -468,6 +472,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -643,11 +648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2432,15 +2437,18 @@
         <v>0.637972653083412</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:7">
       <c r="B97" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="8" t="s">
         <v>6</v>
       </c>
@@ -2455,6 +2463,12 @@
       </c>
       <c r="E98" s="8">
         <v>0.88218205602480104</v>
+      </c>
+      <c r="F98">
+        <v>0.879535047551954</v>
+      </c>
+      <c r="G98">
+        <v>0.87966749924717902</v>
       </c>
     </row>
   </sheetData>
@@ -2474,7 +2488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>